<commit_message>
xlsx highlighted errors check
</commit_message>
<xml_diff>
--- a/rules/CORE-000002/negative/01/data/unit-test-coreid-CG0208-negative01.xlsx
+++ b/rules/CORE-000002/negative/01/data/unit-test-coreid-CG0208-negative01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11214"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dbooth/Downloads/cg0208/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rich/Documents/github/core-contributor/rules/CORE-000002/negative/01/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{03423806-4B44-3A46-AAAB-3114AAAEFE94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B10B17DD-43D3-584C-AB73-79FF327CEC87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36940" yWindow="6580" windowWidth="17280" windowHeight="9040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="30240" windowHeight="18980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datasets" sheetId="2" r:id="rId1"/>
@@ -372,7 +372,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -389,23 +389,26 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="3" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="3" xfId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -416,6 +419,12 @@
     <cellStyle name="Note" xfId="3" builtinId="10"/>
   </cellStyles>
   <dxfs count="19">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -519,12 +528,6 @@
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -545,30 +548,30 @@
     <sortCondition ref="A2:A63"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Filename" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Label" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Filename" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Label" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F8F8C63C-3A20-4734-A8F9-B8B0DB6847B7}" name="Table3867" displayName="Table3867" ref="A1:M12" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F8F8C63C-3A20-4734-A8F9-B8B0DB6847B7}" name="Table3867" displayName="Table3867" ref="A1:M12" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
   <autoFilter ref="A1:M12" xr:uid="{F8F8C63C-3A20-4734-A8F9-B8B0DB6847B7}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{6517045E-8B32-4C8E-B093-046C70C35775}" name="STUDYID" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{F90B7898-9F26-4C8E-B615-D0BCA7F37413}" name="DOMAIN" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{2752F126-3558-4C68-A79C-5D13E324FD14}" name="USUBJID" dataDxfId="10"/>
-    <tableColumn id="24" xr3:uid="{B026024E-77E6-4E08-946D-F7EBCE080282}" name="SESEQ" dataDxfId="9"/>
-    <tableColumn id="25" xr3:uid="{8EB8379E-7C31-4384-9E00-F905D362A1A8}" name="ETCD" dataDxfId="8"/>
-    <tableColumn id="26" xr3:uid="{FEEE5B66-B7DF-42F5-BFBA-3931AF14E163}" name="ELEMENT" dataDxfId="7"/>
-    <tableColumn id="27" xr3:uid="{CE0DD070-C039-446E-9DD3-16B8EDFBCD2B}" name="TAETORD" dataDxfId="6"/>
-    <tableColumn id="28" xr3:uid="{957042EA-C19F-4BA3-B31D-D7F0AE2F102F}" name="EPOCH" dataDxfId="5"/>
-    <tableColumn id="29" xr3:uid="{D6379F26-837D-4FE2-B2AC-EAA7FC625C19}" name="SESTDTC" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{5631B557-4872-4970-A6BA-7865CC8B51E6}" name="SEENDTC" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{6C229BA1-D693-4634-97B1-0CB13E2B03C0}" name="SESTDY" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{5E70737F-7845-4ABD-916B-CF6B87ACE3E9}" name="SEENDY" dataDxfId="1" dataCellStyle="Normal 3"/>
-    <tableColumn id="6" xr3:uid="{6C44C455-7520-4E4F-A775-9CA02A5B15CB}" name="SEUPDES" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{6517045E-8B32-4C8E-B093-046C70C35775}" name="STUDYID" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{F90B7898-9F26-4C8E-B615-D0BCA7F37413}" name="DOMAIN" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{2752F126-3558-4C68-A79C-5D13E324FD14}" name="USUBJID" dataDxfId="12"/>
+    <tableColumn id="24" xr3:uid="{B026024E-77E6-4E08-946D-F7EBCE080282}" name="SESEQ" dataDxfId="11"/>
+    <tableColumn id="25" xr3:uid="{8EB8379E-7C31-4384-9E00-F905D362A1A8}" name="ETCD" dataDxfId="10"/>
+    <tableColumn id="26" xr3:uid="{FEEE5B66-B7DF-42F5-BFBA-3931AF14E163}" name="ELEMENT" dataDxfId="9"/>
+    <tableColumn id="27" xr3:uid="{CE0DD070-C039-446E-9DD3-16B8EDFBCD2B}" name="TAETORD" dataDxfId="8"/>
+    <tableColumn id="28" xr3:uid="{957042EA-C19F-4BA3-B31D-D7F0AE2F102F}" name="EPOCH" dataDxfId="7"/>
+    <tableColumn id="29" xr3:uid="{D6379F26-837D-4FE2-B2AC-EAA7FC625C19}" name="SESTDTC" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{5631B557-4872-4970-A6BA-7865CC8B51E6}" name="SEENDTC" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{6C229BA1-D693-4634-97B1-0CB13E2B03C0}" name="SESTDY" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{5E70737F-7845-4ABD-916B-CF6B87ACE3E9}" name="SEENDY" dataDxfId="3" dataCellStyle="Normal 3"/>
+    <tableColumn id="6" xr3:uid="{6C44C455-7520-4E4F-A775-9CA02A5B15CB}" name="SEUPDES" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -840,7 +843,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -877,8 +880,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A6B7066-B3A9-471E-B8AC-560BE7C34DF3}">
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1229,7 +1232,7 @@
       <c r="H9" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="I9" s="11"/>
+      <c r="I9" s="12"/>
       <c r="J9" s="10" t="s">
         <v>35</v>
       </c>
@@ -1365,6 +1368,7 @@
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -1381,6 +1385,14 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Comment xmlns="9dee18c2-6da5-44c1-913e-bf7f393fe0e8" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010090ADB40D834AE945B19FCDA4041AC0CB" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d8944bc5b49d53466ed9616bc741861d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9dee18c2-6da5-44c1-913e-bf7f393fe0e8" xmlns:ns3="63ea592b-d684-45c7-8cdc-fad8f8e6bb41" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a3663bc803fcda44b1cdcfc700c45575" ns2:_="" ns3:_="">
     <xsd:import namespace="9dee18c2-6da5-44c1-913e-bf7f393fe0e8"/>
@@ -1567,14 +1579,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Comment xmlns="9dee18c2-6da5-44c1-913e-bf7f393fe0e8" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CE37091-6FF4-4182-990E-B7D3ED1B8142}">
   <ds:schemaRefs>
@@ -1584,14 +1588,30 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2457BC1C-7D32-4C16-8AC3-7A58D1590D4A}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C96795B8-EDF4-4988-AD31-61F6ECF896A9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9dee18c2-6da5-44c1-913e-bf7f393fe0e8"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2457BC1C-7D32-4C16-8AC3-7A58D1590D4A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="9dee18c2-6da5-44c1-913e-bf7f393fe0e8"/>
+    <ds:schemaRef ds:uri="63ea592b-d684-45c7-8cdc-fad8f8e6bb41"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>